<commit_message>
add attributes to contract class
</commit_message>
<xml_diff>
--- a/test files/test.xlsx
+++ b/test files/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="statment" sheetId="6" r:id="rId1"/>
@@ -150,10 +150,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -784,7 +785,7 @@
     <xf numFmtId="43" fontId="11" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="11" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1131,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2657,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3281,7 +3282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish oneContractDates function in Invoice
</commit_message>
<xml_diff>
--- a/test files/test.xlsx
+++ b/test files/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="statment" sheetId="6" r:id="rId1"/>
@@ -150,11 +150,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -592,7 +591,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -785,9 +784,6 @@
     <xf numFmtId="43" fontId="11" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="11" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1132,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1214,18 +1210,18 @@
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="30"/>
-      <c r="H2" s="72">
-        <v>45230</v>
+      <c r="H2" s="31">
+        <v>44870</v>
       </c>
       <c r="I2" s="31">
-        <v>45235</v>
+        <v>45601</v>
       </c>
       <c r="J2" s="31" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="28">
         <f t="shared" ref="K2:K30" si="0">+I2-H2</f>
-        <v>5</v>
+        <v>731</v>
       </c>
       <c r="L2" s="67">
         <v>54</v>
@@ -2659,7 +2655,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3282,7 +3278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
do allContractsDates functions, compute nights * rate code without offers
</commit_message>
<xml_diff>
--- a/test files/test.xlsx
+++ b/test files/test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="37">
   <si>
     <t>Net Amount.</t>
   </si>
@@ -150,10 +150,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -591,7 +592,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -784,6 +785,9 @@
     <xf numFmtId="43" fontId="11" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="11" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1126,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1210,18 +1214,18 @@
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="30"/>
-      <c r="H2" s="31">
-        <v>44870</v>
+      <c r="H2" s="72">
+        <v>45230</v>
       </c>
       <c r="I2" s="31">
-        <v>45601</v>
+        <v>45235</v>
       </c>
       <c r="J2" s="31" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="28">
         <f t="shared" ref="K2:K30" si="0">+I2-H2</f>
-        <v>731</v>
+        <v>5</v>
       </c>
       <c r="L2" s="67">
         <v>54</v>
@@ -1945,7 +1949,7 @@
         <v>8145.482456140352</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="15">
+    <row r="17" spans="1:17" ht="15">
       <c r="B17" s="12">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -1995,7 +1999,7 @@
         <v>10229.210526315792</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="15">
+    <row r="18" spans="1:17" ht="15">
       <c r="B18" s="12">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -2045,7 +2049,7 @@
         <v>7577.1929824561412</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="15">
+    <row r="19" spans="1:17" ht="15">
       <c r="B19" s="12">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -2095,7 +2099,7 @@
         <v>8145.482456140352</v>
       </c>
     </row>
-    <row r="20" spans="2:17" ht="15">
+    <row r="20" spans="1:17" ht="15">
       <c r="B20" s="12">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -2145,7 +2149,7 @@
         <v>6494.7368421052633</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="15">
+    <row r="21" spans="1:17" ht="15">
       <c r="B21" s="12">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -2195,7 +2199,7 @@
         <v>10229.210526315792</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="15">
+    <row r="22" spans="1:17" ht="15">
       <c r="B22" s="12">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -2245,7 +2249,7 @@
         <v>9471.4912280701756</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="15">
+    <row r="23" spans="1:17" ht="15">
       <c r="B23" s="12">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -2295,7 +2299,7 @@
         <v>9471.4912280701756</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="15">
+    <row r="24" spans="1:17" ht="15">
       <c r="B24" s="12">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -2345,7 +2349,7 @@
         <v>8145.482456140352</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="15">
+    <row r="25" spans="1:17" ht="15">
       <c r="B25" s="12">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -2395,7 +2399,7 @@
         <v>10229.210526315792</v>
       </c>
     </row>
-    <row r="26" spans="2:17" ht="15">
+    <row r="26" spans="1:17" ht="15">
       <c r="B26" s="12">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -2445,7 +2449,7 @@
         <v>10824.561403508773</v>
       </c>
     </row>
-    <row r="27" spans="2:17" ht="15">
+    <row r="27" spans="1:17" ht="15">
       <c r="B27" s="12">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -2495,7 +2499,7 @@
         <v>9471.4912280701756</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="15">
+    <row r="28" spans="1:17" ht="15">
       <c r="B28" s="12">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -2545,7 +2549,7 @@
         <v>8767.894736842105</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="15">
+    <row r="29" spans="1:17" ht="15">
       <c r="B29" s="12">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -2595,7 +2599,7 @@
         <v>17860.526315789477</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="15">
+    <row r="30" spans="1:17" ht="15.75" thickBot="1">
       <c r="B30" s="12">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -2645,6 +2649,57 @@
         <v>11690.526315789475</v>
       </c>
     </row>
+    <row r="31" spans="1:17" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16">
+        <v>1</v>
+      </c>
+      <c r="C31" s="41">
+        <v>45229</v>
+      </c>
+      <c r="D31" s="27">
+        <v>116303569264</v>
+      </c>
+      <c r="E31" s="28">
+        <v>161333</v>
+      </c>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="52">
+        <v>45336</v>
+      </c>
+      <c r="I31" s="55">
+        <v>45412</v>
+      </c>
+      <c r="J31" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="28">
+        <f t="shared" ref="K31" si="4">+I31-H31</f>
+        <v>76</v>
+      </c>
+      <c r="L31" s="67">
+        <v>54</v>
+      </c>
+      <c r="M31" s="68">
+        <v>260</v>
+      </c>
+      <c r="N31" s="69">
+        <v>30.85</v>
+      </c>
+      <c r="O31" s="67">
+        <v>8329.5</v>
+      </c>
+      <c r="P31" s="32">
+        <f t="shared" ref="P31" si="5">+O31-Q31</f>
+        <v>1022.9210526315783</v>
+      </c>
+      <c r="Q31" s="33">
+        <f t="shared" ref="Q31" si="6">+O31/1.14</f>
+        <v>7306.5789473684217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="13.5" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2655,7 +2710,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3607,7 +3662,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
finish codes with offers
</commit_message>
<xml_diff>
--- a/test files/test.xlsx
+++ b/test files/test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
   <si>
     <t>Net Amount.</t>
   </si>
@@ -131,30 +131,17 @@
     <t>13/11/2023</t>
   </si>
   <si>
-    <t>17/11/2023</t>
-  </si>
-  <si>
-    <t>18/11/2023</t>
-  </si>
-  <si>
-    <t>19/11/2023</t>
-  </si>
-  <si>
-    <t>20/11/2023</t>
-  </si>
-  <si>
-    <t>21/11/2023</t>
+    <t>sk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -785,7 +772,7 @@
     <xf numFmtId="43" fontId="11" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="11" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1132,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1215,17 +1202,17 @@
       <c r="F2" s="29"/>
       <c r="G2" s="30"/>
       <c r="H2" s="72">
-        <v>45230</v>
+        <v>0</v>
       </c>
       <c r="I2" s="31">
-        <v>45235</v>
+        <v>0</v>
       </c>
       <c r="J2" s="31" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="28">
         <f t="shared" ref="K2:K30" si="0">+I2-H2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L2" s="67">
         <v>54</v>
@@ -1270,9 +1257,7 @@
       <c r="I3" s="29">
         <v>45235</v>
       </c>
-      <c r="J3" s="29" t="s">
-        <v>23</v>
-      </c>
+      <c r="J3" s="29"/>
       <c r="K3" s="35">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1318,15 +1303,13 @@
       <c r="H4" s="29">
         <v>45230</v>
       </c>
-      <c r="I4" s="29">
-        <v>45235</v>
-      </c>
+      <c r="I4" s="29"/>
       <c r="J4" s="29" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="35">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-45230</v>
       </c>
       <c r="L4" s="71">
         <v>54</v>
@@ -1365,9 +1348,7 @@
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="29">
-        <v>45233</v>
-      </c>
+      <c r="H5" s="29"/>
       <c r="I5" s="29">
         <v>45239</v>
       </c>
@@ -1376,7 +1357,7 @@
       </c>
       <c r="K5" s="35">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>45239</v>
       </c>
       <c r="L5" s="71">
         <v>54</v>
@@ -1504,9 +1485,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="C8" s="41">
-        <v>45229</v>
-      </c>
+      <c r="C8" s="41"/>
       <c r="D8" s="34">
         <v>115363600331</v>
       </c>
@@ -1555,48 +1534,48 @@
         <v>8</v>
       </c>
       <c r="C9" s="41">
-        <v>45237</v>
+        <v>45229</v>
       </c>
       <c r="D9" s="34">
-        <v>116383610193</v>
+        <v>116383606590</v>
       </c>
       <c r="E9" s="35">
-        <v>161910</v>
+        <v>161753</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="36"/>
       <c r="H9" s="29">
-        <v>45240</v>
-      </c>
-      <c r="I9" s="29" t="s">
+        <v>45237</v>
+      </c>
+      <c r="I9" s="29">
+        <v>45244</v>
+      </c>
+      <c r="J9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="K9" s="35">
+        <f t="shared" ref="K9:K10" si="4">+I9-H9</f>
+        <v>7</v>
       </c>
       <c r="L9" s="71">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="M9" s="68">
-        <v>350</v>
+        <v>378</v>
       </c>
       <c r="N9" s="70">
         <v>30.85</v>
       </c>
       <c r="O9" s="68">
-        <v>10797.5</v>
+        <v>11661.300000000001</v>
       </c>
       <c r="P9" s="37">
-        <f t="shared" si="1"/>
-        <v>1326.0087719298244</v>
+        <f t="shared" ref="P9:P10" si="5">+O9-Q9</f>
+        <v>1432.0894736842092</v>
       </c>
       <c r="Q9" s="38">
-        <f t="shared" si="2"/>
-        <v>9471.4912280701756</v>
+        <f t="shared" ref="Q9:Q10" si="6">+O9/1.14</f>
+        <v>10229.210526315792</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15">
@@ -1605,1099 +1584,428 @@
         <v>9</v>
       </c>
       <c r="C10" s="41">
-        <v>45231</v>
+        <v>46325</v>
       </c>
       <c r="D10" s="34">
-        <v>116353608470</v>
+        <v>115363600331</v>
       </c>
       <c r="E10" s="35">
-        <v>161911</v>
+        <v>161799</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="36"/>
       <c r="H10" s="29">
-        <v>45240</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>32</v>
+        <v>45238</v>
+      </c>
+      <c r="I10" s="29">
+        <v>45245</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>21</v>
+      </c>
+      <c r="K10" s="35">
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="L10" s="71">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="M10" s="68">
-        <v>378</v>
+        <v>301</v>
       </c>
       <c r="N10" s="70">
         <v>30.85</v>
       </c>
       <c r="O10" s="68">
-        <v>11661.300000000001</v>
+        <v>9285.85</v>
       </c>
       <c r="P10" s="37">
-        <f t="shared" si="1"/>
-        <v>1432.0894736842092</v>
+        <f t="shared" si="5"/>
+        <v>1140.3675438596483</v>
       </c>
       <c r="Q10" s="38">
-        <f t="shared" si="2"/>
-        <v>10229.210526315792</v>
+        <f t="shared" si="6"/>
+        <v>8145.482456140352</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15">
-      <c r="B11" s="12">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="C11" s="41">
-        <v>45234</v>
-      </c>
-      <c r="D11" s="34">
-        <v>115363600416</v>
-      </c>
-      <c r="E11" s="35">
-        <v>161913</v>
-      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="29"/>
       <c r="G11" s="36"/>
-      <c r="H11" s="29">
-        <v>45240</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L11" s="71">
-        <v>50</v>
-      </c>
-      <c r="M11" s="68">
-        <v>350</v>
-      </c>
-      <c r="N11" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O11" s="68">
-        <v>10797.5</v>
-      </c>
-      <c r="P11" s="37">
-        <f t="shared" si="1"/>
-        <v>1326.0087719298244</v>
-      </c>
-      <c r="Q11" s="38">
-        <f t="shared" si="2"/>
-        <v>9471.4912280701756</v>
-      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="38"/>
     </row>
     <row r="12" spans="1:17" ht="15">
-      <c r="B12" s="12">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="C12" s="41">
-        <v>45234</v>
-      </c>
-      <c r="D12" s="34">
-        <v>115363600416</v>
-      </c>
-      <c r="E12" s="35">
-        <v>161914</v>
-      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="29"/>
       <c r="G12" s="36"/>
-      <c r="H12" s="29">
-        <v>45240</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L12" s="71">
-        <v>50</v>
-      </c>
-      <c r="M12" s="68">
-        <v>350</v>
-      </c>
-      <c r="N12" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O12" s="68">
-        <v>10797.5</v>
-      </c>
-      <c r="P12" s="37">
-        <f t="shared" si="1"/>
-        <v>1326.0087719298244</v>
-      </c>
-      <c r="Q12" s="38">
-        <f t="shared" si="2"/>
-        <v>9471.4912280701756</v>
-      </c>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="38"/>
     </row>
     <row r="13" spans="1:17" ht="15">
-      <c r="B13" s="12">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="C13" s="41">
-        <v>45231</v>
-      </c>
-      <c r="D13" s="34">
-        <v>116383608640</v>
-      </c>
-      <c r="E13" s="35">
-        <v>161916</v>
-      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="29"/>
       <c r="G13" s="36"/>
-      <c r="H13" s="29">
-        <v>45240</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L13" s="71">
-        <v>54</v>
-      </c>
-      <c r="M13" s="68">
-        <v>378</v>
-      </c>
-      <c r="N13" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O13" s="68">
-        <v>11661.300000000001</v>
-      </c>
-      <c r="P13" s="37">
-        <f t="shared" si="1"/>
-        <v>1432.0894736842092</v>
-      </c>
-      <c r="Q13" s="38">
-        <f t="shared" si="2"/>
-        <v>10229.210526315792</v>
-      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="38"/>
     </row>
     <row r="14" spans="1:17" ht="15">
-      <c r="B14" s="12">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="C14" s="41">
-        <v>45236</v>
-      </c>
-      <c r="D14" s="34">
-        <v>116323611002</v>
-      </c>
-      <c r="E14" s="35">
-        <v>161980</v>
-      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="29"/>
       <c r="G14" s="36"/>
-      <c r="H14" s="29">
-        <v>45241</v>
-      </c>
-      <c r="I14" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L14" s="71">
-        <v>129</v>
-      </c>
-      <c r="M14" s="68">
-        <v>903</v>
-      </c>
-      <c r="N14" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O14" s="68">
-        <v>27857.550000000003</v>
-      </c>
-      <c r="P14" s="37">
-        <f t="shared" si="1"/>
-        <v>3421.1026315789459</v>
-      </c>
-      <c r="Q14" s="38">
-        <f t="shared" si="2"/>
-        <v>24436.447368421057</v>
-      </c>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="68"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="38"/>
     </row>
     <row r="15" spans="1:17" ht="15">
-      <c r="B15" s="12">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="C15" s="41">
-        <v>45234</v>
-      </c>
-      <c r="D15" s="34">
-        <v>116383609128</v>
-      </c>
-      <c r="E15" s="35">
-        <v>162029</v>
-      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="29"/>
       <c r="G15" s="36"/>
-      <c r="H15" s="29">
-        <v>45241</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L15" s="71">
-        <v>50</v>
-      </c>
-      <c r="M15" s="68">
-        <v>350</v>
-      </c>
-      <c r="N15" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O15" s="68">
-        <v>10797.5</v>
-      </c>
-      <c r="P15" s="37">
-        <f t="shared" si="1"/>
-        <v>1326.0087719298244</v>
-      </c>
-      <c r="Q15" s="38">
-        <f t="shared" si="2"/>
-        <v>9471.4912280701756</v>
-      </c>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="70"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="38"/>
     </row>
     <row r="16" spans="1:17" ht="15">
-      <c r="B16" s="12">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="C16" s="41">
-        <v>45232</v>
-      </c>
-      <c r="D16" s="34">
-        <v>116383608138</v>
-      </c>
-      <c r="E16" s="35">
-        <v>162033</v>
-      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="29"/>
       <c r="G16" s="36"/>
-      <c r="H16" s="29">
-        <v>45241</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L16" s="71">
-        <v>43</v>
-      </c>
-      <c r="M16" s="68">
-        <v>301</v>
-      </c>
-      <c r="N16" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O16" s="68">
-        <v>9285.85</v>
-      </c>
-      <c r="P16" s="37">
-        <f t="shared" si="1"/>
-        <v>1140.3675438596483</v>
-      </c>
-      <c r="Q16" s="38">
-        <f t="shared" si="2"/>
-        <v>8145.482456140352</v>
-      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="38"/>
     </row>
     <row r="17" spans="1:17" ht="15">
-      <c r="B17" s="12">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="C17" s="41">
-        <v>45233</v>
-      </c>
-      <c r="D17" s="34">
-        <v>116323609306</v>
-      </c>
-      <c r="E17" s="35">
-        <v>162077</v>
-      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="29"/>
       <c r="G17" s="36"/>
-      <c r="H17" s="29">
-        <v>45242</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L17" s="71">
-        <v>54</v>
-      </c>
-      <c r="M17" s="68">
-        <v>378</v>
-      </c>
-      <c r="N17" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O17" s="68">
-        <v>11661.300000000001</v>
-      </c>
-      <c r="P17" s="37">
-        <f t="shared" si="1"/>
-        <v>1432.0894736842092</v>
-      </c>
-      <c r="Q17" s="38">
-        <f t="shared" si="2"/>
-        <v>10229.210526315792</v>
-      </c>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="38"/>
     </row>
     <row r="18" spans="1:17" ht="15">
-      <c r="B18" s="12">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="C18" s="41">
-        <v>45238</v>
-      </c>
-      <c r="D18" s="34">
-        <v>116373610741</v>
-      </c>
-      <c r="E18" s="35">
-        <v>162079</v>
-      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="29"/>
       <c r="G18" s="36"/>
-      <c r="H18" s="29">
-        <v>45242</v>
-      </c>
-      <c r="I18" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L18" s="71">
-        <v>40</v>
-      </c>
-      <c r="M18" s="68">
-        <v>280</v>
-      </c>
-      <c r="N18" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O18" s="68">
-        <v>8638</v>
-      </c>
-      <c r="P18" s="37">
-        <f t="shared" si="1"/>
-        <v>1060.8070175438588</v>
-      </c>
-      <c r="Q18" s="38">
-        <f t="shared" si="2"/>
-        <v>7577.1929824561412</v>
-      </c>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="38"/>
     </row>
     <row r="19" spans="1:17" ht="15">
-      <c r="B19" s="12">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="C19" s="41">
-        <v>45231</v>
-      </c>
-      <c r="D19" s="34">
-        <v>116323608224</v>
-      </c>
-      <c r="E19" s="35">
-        <v>162080</v>
-      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="29"/>
       <c r="G19" s="36"/>
-      <c r="H19" s="29">
-        <v>45242</v>
-      </c>
-      <c r="I19" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L19" s="71">
-        <v>43</v>
-      </c>
-      <c r="M19" s="68">
-        <v>301</v>
-      </c>
-      <c r="N19" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O19" s="68">
-        <v>9285.85</v>
-      </c>
-      <c r="P19" s="37">
-        <f t="shared" si="1"/>
-        <v>1140.3675438596483</v>
-      </c>
-      <c r="Q19" s="38">
-        <f t="shared" si="2"/>
-        <v>8145.482456140352</v>
-      </c>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="68"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="38"/>
     </row>
     <row r="20" spans="1:17" ht="15">
-      <c r="B20" s="12">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="C20" s="41">
-        <v>45237</v>
-      </c>
-      <c r="D20" s="34">
-        <v>116353610541</v>
-      </c>
-      <c r="E20" s="35">
-        <v>162132</v>
-      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="29"/>
       <c r="G20" s="36"/>
-      <c r="H20" s="29">
-        <v>45244</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L20" s="71">
-        <v>40</v>
-      </c>
-      <c r="M20" s="68">
-        <v>240</v>
-      </c>
-      <c r="N20" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O20" s="68">
-        <v>7404</v>
-      </c>
-      <c r="P20" s="37">
-        <f t="shared" si="1"/>
-        <v>909.26315789473665</v>
-      </c>
-      <c r="Q20" s="38">
-        <f t="shared" si="2"/>
-        <v>6494.7368421052633</v>
-      </c>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="68"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="38"/>
     </row>
     <row r="21" spans="1:17" ht="15">
-      <c r="B21" s="12">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="C21" s="41">
-        <v>45230</v>
-      </c>
-      <c r="D21" s="34">
-        <v>116373607505</v>
-      </c>
-      <c r="E21" s="35">
-        <v>162154</v>
-      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
       <c r="F21" s="29"/>
       <c r="G21" s="36"/>
-      <c r="H21" s="29">
-        <v>45243</v>
-      </c>
-      <c r="I21" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L21" s="71">
-        <v>54</v>
-      </c>
-      <c r="M21" s="68">
-        <v>378</v>
-      </c>
-      <c r="N21" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O21" s="68">
-        <v>11661.300000000001</v>
-      </c>
-      <c r="P21" s="37">
-        <f t="shared" si="1"/>
-        <v>1432.0894736842092</v>
-      </c>
-      <c r="Q21" s="38">
-        <f t="shared" si="2"/>
-        <v>10229.210526315792</v>
-      </c>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="38"/>
     </row>
     <row r="22" spans="1:17" ht="15">
-      <c r="B22" s="12">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="C22" s="41">
-        <v>45237</v>
-      </c>
-      <c r="D22" s="34">
-        <v>116373611410</v>
-      </c>
-      <c r="E22" s="35">
-        <v>162159</v>
-      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
       <c r="F22" s="29"/>
       <c r="G22" s="36"/>
-      <c r="H22" s="29">
-        <v>45243</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L22" s="71">
-        <v>50</v>
-      </c>
-      <c r="M22" s="68">
-        <v>350</v>
-      </c>
-      <c r="N22" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O22" s="68">
-        <v>10797.5</v>
-      </c>
-      <c r="P22" s="37">
-        <f t="shared" si="1"/>
-        <v>1326.0087719298244</v>
-      </c>
-      <c r="Q22" s="38">
-        <f t="shared" si="2"/>
-        <v>9471.4912280701756</v>
-      </c>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="68"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="38"/>
     </row>
     <row r="23" spans="1:17" ht="15">
-      <c r="B23" s="12">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="C23" s="41">
-        <v>45237</v>
-      </c>
-      <c r="D23" s="34">
-        <v>116373611410</v>
-      </c>
-      <c r="E23" s="35">
-        <v>162165</v>
-      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="35"/>
       <c r="F23" s="29"/>
       <c r="G23" s="36"/>
-      <c r="H23" s="29">
-        <v>45243</v>
-      </c>
-      <c r="I23" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L23" s="71">
-        <v>50</v>
-      </c>
-      <c r="M23" s="68">
-        <v>350</v>
-      </c>
-      <c r="N23" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O23" s="68">
-        <v>10797.5</v>
-      </c>
-      <c r="P23" s="37">
-        <f t="shared" si="1"/>
-        <v>1326.0087719298244</v>
-      </c>
-      <c r="Q23" s="38">
-        <f t="shared" si="2"/>
-        <v>9471.4912280701756</v>
-      </c>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="68"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="38"/>
     </row>
     <row r="24" spans="1:17" ht="15">
-      <c r="B24" s="12">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="C24" s="41">
-        <v>45233</v>
-      </c>
-      <c r="D24" s="34">
-        <v>116323610067</v>
-      </c>
-      <c r="E24" s="35">
-        <v>162175</v>
-      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
       <c r="F24" s="29"/>
       <c r="G24" s="36"/>
-      <c r="H24" s="29">
-        <v>45244</v>
-      </c>
-      <c r="I24" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J24" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L24" s="71">
-        <v>43</v>
-      </c>
-      <c r="M24" s="68">
-        <v>301</v>
-      </c>
-      <c r="N24" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O24" s="68">
-        <v>9285.85</v>
-      </c>
-      <c r="P24" s="37">
-        <f t="shared" si="1"/>
-        <v>1140.3675438596483</v>
-      </c>
-      <c r="Q24" s="38">
-        <f t="shared" si="2"/>
-        <v>8145.482456140352</v>
-      </c>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="38"/>
     </row>
     <row r="25" spans="1:17" ht="15">
-      <c r="B25" s="12">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="C25" s="41">
-        <v>45234</v>
-      </c>
-      <c r="D25" s="34">
-        <v>116363608907</v>
-      </c>
-      <c r="E25" s="35">
-        <v>162176</v>
-      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35"/>
       <c r="F25" s="29"/>
       <c r="G25" s="36"/>
-      <c r="H25" s="29">
-        <v>45244</v>
-      </c>
-      <c r="I25" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L25" s="71">
-        <v>54</v>
-      </c>
-      <c r="M25" s="68">
-        <v>378</v>
-      </c>
-      <c r="N25" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O25" s="68">
-        <v>11661.300000000001</v>
-      </c>
-      <c r="P25" s="37">
-        <f t="shared" si="1"/>
-        <v>1432.0894736842092</v>
-      </c>
-      <c r="Q25" s="38">
-        <f t="shared" si="2"/>
-        <v>10229.210526315792</v>
-      </c>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="38"/>
     </row>
     <row r="26" spans="1:17" ht="15">
-      <c r="B26" s="12">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="C26" s="41">
-        <v>45237</v>
-      </c>
-      <c r="D26" s="34">
-        <v>116353610398</v>
-      </c>
-      <c r="E26" s="35">
-        <v>162177</v>
-      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35"/>
       <c r="F26" s="29"/>
       <c r="G26" s="36"/>
-      <c r="H26" s="29">
-        <v>45243</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K26" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L26" s="71">
-        <v>50</v>
-      </c>
-      <c r="M26" s="68">
-        <v>400</v>
-      </c>
-      <c r="N26" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O26" s="68">
-        <v>12340</v>
-      </c>
-      <c r="P26" s="37">
-        <f t="shared" si="1"/>
-        <v>1515.4385964912271</v>
-      </c>
-      <c r="Q26" s="38">
-        <f t="shared" si="2"/>
-        <v>10824.561403508773</v>
-      </c>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="70"/>
+      <c r="O26" s="68"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="38"/>
     </row>
     <row r="27" spans="1:17" ht="15">
-      <c r="B27" s="12">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="C27" s="41">
-        <v>45238</v>
-      </c>
-      <c r="D27" s="34">
-        <v>116363611495</v>
-      </c>
-      <c r="E27" s="35">
-        <v>162182</v>
-      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="35"/>
       <c r="F27" s="29"/>
       <c r="G27" s="36"/>
-      <c r="H27" s="29">
-        <v>45244</v>
-      </c>
-      <c r="I27" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J27" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L27" s="71">
-        <v>50</v>
-      </c>
-      <c r="M27" s="68">
-        <v>350</v>
-      </c>
-      <c r="N27" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O27" s="68">
-        <v>10797.5</v>
-      </c>
-      <c r="P27" s="37">
-        <f t="shared" si="1"/>
-        <v>1326.0087719298244</v>
-      </c>
-      <c r="Q27" s="38">
-        <f t="shared" si="2"/>
-        <v>9471.4912280701756</v>
-      </c>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="68"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="38"/>
     </row>
     <row r="28" spans="1:17" ht="15">
-      <c r="B28" s="12">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="C28" s="41">
-        <v>45234</v>
-      </c>
-      <c r="D28" s="34">
-        <v>116383610612</v>
-      </c>
-      <c r="E28" s="35">
-        <v>162183</v>
-      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
       <c r="F28" s="29"/>
       <c r="G28" s="36"/>
-      <c r="H28" s="29">
-        <v>45245</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J28" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L28" s="71">
-        <v>54</v>
-      </c>
-      <c r="M28" s="68">
-        <v>324</v>
-      </c>
-      <c r="N28" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O28" s="68">
-        <v>9995.4</v>
-      </c>
-      <c r="P28" s="37">
-        <f t="shared" si="1"/>
-        <v>1227.5052631578947</v>
-      </c>
-      <c r="Q28" s="38">
-        <f t="shared" si="2"/>
-        <v>8767.894736842105</v>
-      </c>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="68"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="38"/>
     </row>
     <row r="29" spans="1:17" ht="15">
-      <c r="B29" s="12">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="C29" s="41">
-        <v>45232</v>
-      </c>
-      <c r="D29" s="34">
-        <v>116363609218</v>
-      </c>
-      <c r="E29" s="35">
-        <v>162197</v>
-      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="35"/>
       <c r="F29" s="29"/>
       <c r="G29" s="36"/>
-      <c r="H29" s="29">
-        <v>45241</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L29" s="71">
-        <v>66</v>
-      </c>
-      <c r="M29" s="68">
-        <v>660</v>
-      </c>
-      <c r="N29" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O29" s="68">
-        <v>20361</v>
-      </c>
-      <c r="P29" s="37">
-        <f t="shared" si="1"/>
-        <v>2500.4736842105231</v>
-      </c>
-      <c r="Q29" s="38">
-        <f t="shared" si="2"/>
-        <v>17860.526315789477</v>
-      </c>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="38"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" thickBot="1">
-      <c r="B30" s="12">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="C30" s="41">
-        <v>45236</v>
-      </c>
-      <c r="D30" s="34">
-        <v>116343610274</v>
-      </c>
-      <c r="E30" s="35">
-        <v>162201</v>
-      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="35"/>
       <c r="F30" s="29"/>
       <c r="G30" s="36"/>
-      <c r="H30" s="29">
-        <v>45243</v>
-      </c>
-      <c r="I30" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J30" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L30" s="71">
-        <v>54</v>
-      </c>
-      <c r="M30" s="68">
-        <v>400</v>
-      </c>
-      <c r="N30" s="70">
-        <v>30.85</v>
-      </c>
-      <c r="O30" s="68">
-        <v>13327.2</v>
-      </c>
-      <c r="P30" s="37">
-        <f t="shared" si="1"/>
-        <v>1636.6736842105256</v>
-      </c>
-      <c r="Q30" s="38">
-        <f t="shared" si="2"/>
-        <v>11690.526315789475</v>
-      </c>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="70"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="38"/>
     </row>
     <row r="31" spans="1:17" ht="16.5" thickTop="1" thickBot="1">
       <c r="A31" s="15"/>
-      <c r="B31" s="16">
-        <v>1</v>
-      </c>
-      <c r="C31" s="41">
-        <v>45229</v>
-      </c>
-      <c r="D31" s="27">
-        <v>116303569264</v>
-      </c>
-      <c r="E31" s="28">
-        <v>161333</v>
-      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
       <c r="F31" s="29"/>
       <c r="G31" s="30"/>
-      <c r="H31" s="52">
-        <v>45336</v>
-      </c>
-      <c r="I31" s="55">
-        <v>45412</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="K31" s="28">
-        <f t="shared" ref="K31" si="4">+I31-H31</f>
-        <v>76</v>
-      </c>
-      <c r="L31" s="67">
-        <v>54</v>
-      </c>
-      <c r="M31" s="68">
-        <v>260</v>
-      </c>
-      <c r="N31" s="69">
-        <v>30.85</v>
-      </c>
-      <c r="O31" s="67">
-        <v>8329.5</v>
-      </c>
-      <c r="P31" s="32">
-        <f t="shared" ref="P31" si="5">+O31-Q31</f>
-        <v>1022.9210526315783</v>
-      </c>
-      <c r="Q31" s="33">
-        <f t="shared" ref="Q31" si="6">+O31/1.14</f>
-        <v>7306.5789473684217</v>
-      </c>
+      <c r="H31" s="52"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="33"/>
     </row>
     <row r="32" spans="1:17" ht="13.5" thickTop="1"/>
   </sheetData>
@@ -2710,7 +2018,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2765,9 +2073,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.25">
-      <c r="A2" s="52">
-        <v>45047</v>
-      </c>
+      <c r="A2" s="52"/>
       <c r="B2" s="52">
         <v>45061</v>
       </c>

</xml_diff>